<commit_message>
corrected Gao PGS. Lifted over PGS to hg38 and recalculated PGS.
</commit_message>
<xml_diff>
--- a/PGS.matching.summary_WCHS_BrCa.xlsx
+++ b/PGS.matching.summary_WCHS_BrCa.xlsx
@@ -487,16 +487,16 @@
         <v>0</v>
       </c>
       <c r="E4" t="n">
-        <v>525</v>
+        <v>44099</v>
       </c>
       <c r="F4" t="n">
-        <v>0.92</v>
+        <v>77.44</v>
       </c>
       <c r="G4" t="n">
-        <v>437</v>
+        <v>39913</v>
       </c>
       <c r="H4" t="n">
-        <v>0.77</v>
+        <v>70.09</v>
       </c>
     </row>
     <row r="5">
@@ -513,16 +513,16 @@
         <v>0</v>
       </c>
       <c r="E5" t="n">
-        <v>271</v>
+        <v>21982</v>
       </c>
       <c r="F5" t="n">
-        <v>0.95</v>
+        <v>77.39</v>
       </c>
       <c r="G5" t="n">
-        <v>220</v>
+        <v>19847</v>
       </c>
       <c r="H5" t="n">
-        <v>0.77</v>
+        <v>69.87</v>
       </c>
     </row>
     <row r="6">
@@ -539,16 +539,16 @@
         <v>0</v>
       </c>
       <c r="E6" t="n">
-        <v>263</v>
+        <v>22685</v>
       </c>
       <c r="F6" t="n">
-        <v>0.9</v>
+        <v>77.4</v>
       </c>
       <c r="G6" t="n">
-        <v>223</v>
+        <v>20553</v>
       </c>
       <c r="H6" t="n">
-        <v>0.76</v>
+        <v>70.13</v>
       </c>
     </row>
     <row r="7">

</xml_diff>

<commit_message>
Added troubleshooting notes and logs for low coverage PGS.
</commit_message>
<xml_diff>
--- a/PGS.matching.summary_WCHS_BrCa.xlsx
+++ b/PGS.matching.summary_WCHS_BrCa.xlsx
@@ -435,16 +435,16 @@
         <v>0</v>
       </c>
       <c r="E2" t="n">
-        <v>224</v>
+        <v>234</v>
       </c>
       <c r="F2" t="n">
-        <v>71.57</v>
+        <v>74.76</v>
       </c>
       <c r="G2" t="n">
-        <v>164</v>
+        <v>172</v>
       </c>
       <c r="H2" t="n">
-        <v>52.4</v>
+        <v>54.95</v>
       </c>
     </row>
     <row r="3">
@@ -461,16 +461,16 @@
         <v>0</v>
       </c>
       <c r="E3" t="n">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="F3" t="n">
-        <v>94.38</v>
+        <v>97.75</v>
       </c>
       <c r="G3" t="n">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="H3" t="n">
-        <v>39.33</v>
+        <v>41.57</v>
       </c>
     </row>
     <row r="4">
@@ -487,16 +487,16 @@
         <v>0</v>
       </c>
       <c r="E4" t="n">
-        <v>44099</v>
+        <v>45386</v>
       </c>
       <c r="F4" t="n">
-        <v>77.44</v>
+        <v>79.7</v>
       </c>
       <c r="G4" t="n">
-        <v>39913</v>
+        <v>41083</v>
       </c>
       <c r="H4" t="n">
-        <v>70.09</v>
+        <v>72.15</v>
       </c>
     </row>
     <row r="5">
@@ -513,16 +513,16 @@
         <v>0</v>
       </c>
       <c r="E5" t="n">
-        <v>21982</v>
+        <v>22608</v>
       </c>
       <c r="F5" t="n">
-        <v>77.39</v>
+        <v>79.59</v>
       </c>
       <c r="G5" t="n">
-        <v>19847</v>
+        <v>20415</v>
       </c>
       <c r="H5" t="n">
-        <v>69.87</v>
+        <v>71.87</v>
       </c>
     </row>
     <row r="6">
@@ -539,16 +539,16 @@
         <v>0</v>
       </c>
       <c r="E6" t="n">
-        <v>22685</v>
+        <v>23370</v>
       </c>
       <c r="F6" t="n">
-        <v>77.4</v>
+        <v>79.74</v>
       </c>
       <c r="G6" t="n">
-        <v>20553</v>
+        <v>21177</v>
       </c>
       <c r="H6" t="n">
-        <v>70.13</v>
+        <v>72.25</v>
       </c>
     </row>
     <row r="7">
@@ -565,10 +565,10 @@
         <v>0</v>
       </c>
       <c r="E7" t="n">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="F7" t="n">
-        <v>84.21</v>
+        <v>86.84</v>
       </c>
       <c r="G7" t="n">
         <v>34</v>

</xml_diff>